<commit_message>
aggiornato con foglio cima
</commit_message>
<xml_diff>
--- a/stat-triennio.xlsx
+++ b/stat-triennio.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiara-sabelli/Dropbox/FISM/2022/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40557F3-0232-194F-A4D8-97B2BE6540AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE564AF-648E-E448-96C4-6ECBF4394BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="740" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{2BB38C0C-134C-A048-A781-F4354465D60F}"/>
+    <workbookView xWindow="7340" yWindow="740" windowWidth="26840" windowHeight="15940" xr2:uid="{2BB38C0C-134C-A048-A781-F4354465D60F}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-2021_it" sheetId="1" r:id="rId1"/>
     <sheet name="2019-2021_fism" sheetId="4" r:id="rId2"/>
-    <sheet name="if" sheetId="5" r:id="rId3"/>
-    <sheet name="stat_it" sheetId="3" r:id="rId4"/>
-    <sheet name="stat_fism" sheetId="2" r:id="rId5"/>
+    <sheet name="num_pub" sheetId="7" r:id="rId3"/>
+    <sheet name="cima" sheetId="8" r:id="rId4"/>
+    <sheet name="altmetric" sheetId="6" r:id="rId5"/>
+    <sheet name="impact_factor" sheetId="5" r:id="rId6"/>
+    <sheet name="stat_it" sheetId="3" r:id="rId7"/>
+    <sheet name="stat_fism" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="41">
   <si>
     <t>any</t>
   </si>
@@ -150,6 +153,18 @@
   </si>
   <si>
     <t>av_if_it</t>
+  </si>
+  <si>
+    <t>av_alt_fism</t>
+  </si>
+  <si>
+    <t>av_alt_it</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>FISM</t>
   </si>
 </sst>
 </file>
@@ -505,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15BA99C-C1A5-0D45-8D00-1E8A8238F54F}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1490,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1886553-593B-F44B-AFA8-F037AB964ECE}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2472,11 +2487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73F72A7-C305-9649-B4C9-653654303B87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3C1F93-DC02-B44F-BCCF-5322294F7BE6}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2486,10 +2501,10 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,10 +2512,10 @@
         <v>33</v>
       </c>
       <c r="B2">
-        <v>6.2779785474649143</v>
+        <v>293</v>
       </c>
       <c r="C2">
-        <v>5.4585941280129031</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2508,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6.4222222222222225</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>4.844635930786203</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2519,10 +2534,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.9883333333333333</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>4.7525474525474527</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2530,21 +2545,21 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>8.8597908908622163</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>34</v>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>4.5871428571428572</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2552,10 +2567,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4.0856312389900173</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>3.9110339992989838</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2563,10 +2578,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8.0771897289586292</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>6.3226360725720383</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2574,10 +2589,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3.68</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>5.4039411455596431</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2585,10 +2600,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8.8866666666666667</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>5.5444644644644647</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2596,10 +2611,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6.4523076923076923</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>6.152347215934812</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2607,10 +2622,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>4.38</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>4.6858662726265239</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2618,10 +2633,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5.5075896580483734</v>
+        <v>49</v>
       </c>
       <c r="C13">
-        <v>4.6753388345260705</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2629,21 +2644,21 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4.9421833333333334</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>5.2680959276018102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>5.3949999999999996</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2652,6 +2667,546 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C5190-69FF-6742-BDF2-BCCD5876539C}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.9134749524413444</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.8659062591462141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.9843764115432874</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.2481296758104738</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.2512468827930174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.0900628751071735</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.255639097744361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.7624882629107981</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.5920858895705521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.1491904445919046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.5697206303724929</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7765250965250967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.7137718883104589</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.9348286604361371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.9682935271720317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.249283731260411</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.9712073608617593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.7710131758291685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C993833-F6B5-8642-90E2-9B6A7AA9195A}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>14.282157986175285</v>
+      </c>
+      <c r="C2" s="1">
+        <v>14.736020998091083</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>23.372540902995084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.668333333333333</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>67.634465875370921</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>14.002857142857144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.4765217391304351</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.3978343313373252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>16.428571428571427</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14.9970512536055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5.2622772707518468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="C10" s="1">
+        <v>24.818775510204084</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11.250375469336669</v>
+      </c>
+      <c r="C11" s="1">
+        <v>17.738899782135075</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.1039682539682536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>14.618342245989304</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10.455903849191722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.6113671274961598</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12.770288976097039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73F72A7-C305-9649-B4C9-653654303B87}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.2779785474649143</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5.4585941280129031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.4222222222222225</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.844635930786203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.9883333333333333</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.7525474525474527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.8597908908622163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.5871428571428572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.0856312389900173</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.9110339992989838</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.0771897289586292</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6.3226360725720383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3.68</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5.4039411455596431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.8866666666666667</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.5444644644644647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6.4523076923076923</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.152347215934812</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.38</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.6858662726265239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5.5075896580483734</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4.6753388345260705</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.9421833333333334</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5.2680959276018102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.3949999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A8676C-9EDA-6A42-B6C2-E7400D32F918}">
   <dimension ref="A1:Q195"/>
   <sheetViews>
@@ -12455,7 +13010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3674CC-13DA-CC4F-BB28-17C140C0B3A8}">
   <dimension ref="A1:Q195"/>
   <sheetViews>

</xml_diff>

<commit_message>
aggiornamento cima index 2021
</commit_message>
<xml_diff>
--- a/stat-triennio.xlsx
+++ b/stat-triennio.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiara-sabelli/Dropbox/FISM/2022/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE564AF-648E-E448-96C4-6ECBF4394BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8980953F-C928-4540-9C80-34966B4917D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="740" windowWidth="26840" windowHeight="15940" xr2:uid="{2BB38C0C-134C-A048-A781-F4354465D60F}"/>
+    <workbookView xWindow="7340" yWindow="720" windowWidth="26840" windowHeight="15940" activeTab="7" xr2:uid="{2BB38C0C-134C-A048-A781-F4354465D60F}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-2021_it" sheetId="1" r:id="rId1"/>
     <sheet name="2019-2021_fism" sheetId="4" r:id="rId2"/>
-    <sheet name="num_pub" sheetId="7" r:id="rId3"/>
-    <sheet name="cima" sheetId="8" r:id="rId4"/>
-    <sheet name="altmetric" sheetId="6" r:id="rId5"/>
-    <sheet name="impact_factor" sheetId="5" r:id="rId6"/>
-    <sheet name="stat_it" sheetId="3" r:id="rId7"/>
-    <sheet name="stat_fism" sheetId="2" r:id="rId8"/>
+    <sheet name="kw-perc" sheetId="9" r:id="rId3"/>
+    <sheet name="num_pub" sheetId="7" r:id="rId4"/>
+    <sheet name="cima" sheetId="8" r:id="rId5"/>
+    <sheet name="altmetric" sheetId="6" r:id="rId6"/>
+    <sheet name="impact_factor" sheetId="5" r:id="rId7"/>
+    <sheet name="stat_it" sheetId="3" r:id="rId8"/>
+    <sheet name="stat_fism" sheetId="2" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="42">
   <si>
     <t>any</t>
   </si>
@@ -165,6 +166,9 @@
   </si>
   <si>
     <t>FISM</t>
+  </si>
+  <si>
+    <t>altro</t>
   </si>
 </sst>
 </file>
@@ -518,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15BA99C-C1A5-0D45-8D00-1E8A8238F54F}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C16:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,11 +644,11 @@
       </c>
       <c r="P2" s="2">
         <f>(stat_it!$C152*stat_it!P152+stat_it!$C167*stat_it!P167+stat_it!$C182*stat_it!P182)/C2</f>
-        <v>58.505381604696673</v>
+        <v>96.296477495107638</v>
       </c>
       <c r="Q2" s="1">
         <f>(stat_it!$C152*stat_it!P152*stat_it!Q152+stat_it!$C167*stat_it!P167*stat_it!Q167+stat_it!$C182*stat_it!P182*stat_it!Q182)/(stat_it!$C152*stat_it!P152+stat_it!$C167*stat_it!P167+stat_it!$C182*stat_it!P182)</f>
-        <v>1.8659062591462141</v>
+        <v>2.0735200426764213</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -705,11 +709,11 @@
       </c>
       <c r="P3" s="2">
         <f>(stat_it!$C153*stat_it!P153+stat_it!$C168*stat_it!P168+stat_it!$C183*stat_it!P183)/C3</f>
-        <v>68.119658119658126</v>
+        <v>91.247863247863251</v>
       </c>
       <c r="Q3" s="1">
         <f>(stat_it!$C153*stat_it!P153*stat_it!Q153+stat_it!$C168*stat_it!P168*stat_it!Q168+stat_it!$C183*stat_it!P183*stat_it!Q183)/(stat_it!$C153*stat_it!P153+stat_it!$C168*stat_it!P168+stat_it!$C183*stat_it!P183)</f>
-        <v>1.9843764115432874</v>
+        <v>1.9680591982015736</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -770,11 +774,11 @@
       </c>
       <c r="P4" s="2">
         <f>(stat_it!$C154*stat_it!P154+stat_it!$C169*stat_it!P169+stat_it!$C184*stat_it!P184)/C4</f>
-        <v>72.909090909090907</v>
+        <v>81.909090909090907</v>
       </c>
       <c r="Q4" s="1">
         <f>(stat_it!$C154*stat_it!P154*stat_it!Q154+stat_it!$C169*stat_it!P169*stat_it!Q169+stat_it!$C184*stat_it!P184*stat_it!Q184)/(stat_it!$C154*stat_it!P154+stat_it!$C169*stat_it!P169+stat_it!$C184*stat_it!P184)</f>
-        <v>2.2512468827930174</v>
+        <v>2.5560488346281911</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -835,11 +839,11 @@
       </c>
       <c r="P5" s="2">
         <f>(stat_it!$C155*stat_it!P155+stat_it!$C170*stat_it!P170+stat_it!$C185*stat_it!P185)/C5</f>
-        <v>63.618181818181817</v>
+        <v>94.436363636363637</v>
       </c>
       <c r="Q5" s="1">
         <f>(stat_it!$C155*stat_it!P155*stat_it!Q155+stat_it!$C170*stat_it!P170*stat_it!Q170+stat_it!$C185*stat_it!P185*stat_it!Q185)/(stat_it!$C155*stat_it!P155+stat_it!$C170*stat_it!P170+stat_it!$C185*stat_it!P185)</f>
-        <v>2.0900628751071735</v>
+        <v>2.4468194070080864</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -900,11 +904,11 @@
       </c>
       <c r="P6" s="2">
         <f>(stat_it!$C156*stat_it!P156+stat_it!$C171*stat_it!P171+stat_it!$C186*stat_it!P186)/C6</f>
-        <v>57</v>
+        <v>85.857142857142861</v>
       </c>
       <c r="Q6" s="1">
         <f>(stat_it!$C156*stat_it!P156*stat_it!Q156+stat_it!$C171*stat_it!P171*stat_it!Q171+stat_it!$C186*stat_it!P186*stat_it!Q186)/(stat_it!$C156*stat_it!P156+stat_it!$C171*stat_it!P171+stat_it!$C186*stat_it!P186)</f>
-        <v>2.255639097744361</v>
+        <v>2.1680532445923459</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -965,11 +969,11 @@
       </c>
       <c r="P7" s="2">
         <f>(stat_it!$C157*stat_it!P157+stat_it!$C172*stat_it!P172+stat_it!$C187*stat_it!P187)/C7</f>
-        <v>58.214285714285715</v>
+        <v>99</v>
       </c>
       <c r="Q7" s="1">
         <f>(stat_it!$C157*stat_it!P157*stat_it!Q157+stat_it!$C172*stat_it!P172*stat_it!Q172+stat_it!$C187*stat_it!P187*stat_it!Q187)/(stat_it!$C157*stat_it!P157+stat_it!$C172*stat_it!P172+stat_it!$C187*stat_it!P187)</f>
-        <v>1.5920858895705521</v>
+        <v>1.7946464646464648</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1030,11 +1034,11 @@
       </c>
       <c r="P8" s="2">
         <f>(stat_it!$C158*stat_it!P158+stat_it!$C173*stat_it!P173+stat_it!$C188*stat_it!P188)/C8</f>
-        <v>61.510204081632651</v>
+        <v>87.795918367346943</v>
       </c>
       <c r="Q8" s="1">
         <f>(stat_it!$C158*stat_it!P158*stat_it!Q158+stat_it!$C173*stat_it!P173*stat_it!Q173+stat_it!$C188*stat_it!P188*stat_it!Q188)/(stat_it!$C158*stat_it!P158+stat_it!$C173*stat_it!P173+stat_it!$C188*stat_it!P188)</f>
-        <v>2.1491904445919046</v>
+        <v>2.6972524407252441</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1095,11 +1099,11 @@
       </c>
       <c r="P9" s="2">
         <f>(stat_it!$C159*stat_it!P159+stat_it!$C174*stat_it!P174+stat_it!$C189*stat_it!P189)/C9</f>
-        <v>58.166666666666664</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="1">
         <f>(stat_it!$C159*stat_it!P159*stat_it!Q159+stat_it!$C174*stat_it!P174*stat_it!Q174+stat_it!$C189*stat_it!P189*stat_it!Q189)/(stat_it!$C159*stat_it!P159+stat_it!$C174*stat_it!P174+stat_it!$C189*stat_it!P189)</f>
-        <v>1.5697206303724929</v>
+        <v>1.7491666666666668</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1160,11 +1164,11 @@
       </c>
       <c r="P10" s="2">
         <f>(stat_it!$C160*stat_it!P160+stat_it!$C175*stat_it!P175+stat_it!$C190*stat_it!P190)/C10</f>
-        <v>60.941176470588232</v>
+        <v>96.058823529411768</v>
       </c>
       <c r="Q10" s="1">
         <f>(stat_it!$C160*stat_it!P160*stat_it!Q160+stat_it!$C175*stat_it!P175*stat_it!Q175+stat_it!$C190*stat_it!P190*stat_it!Q190)/(stat_it!$C160*stat_it!P160+stat_it!$C175*stat_it!P175+stat_it!$C190*stat_it!P190)</f>
-        <v>1.7765250965250967</v>
+        <v>2.1022229026331907</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1225,11 +1229,11 @@
       </c>
       <c r="P11" s="2">
         <f>(stat_it!$C161*stat_it!P161+stat_it!$C176*stat_it!P176+stat_it!$C191*stat_it!P191)/C11</f>
-        <v>59.614285714285714</v>
+        <v>96.814285714285717</v>
       </c>
       <c r="Q11" s="1">
         <f>(stat_it!$C161*stat_it!P161*stat_it!Q161+stat_it!$C176*stat_it!P176*stat_it!Q176+stat_it!$C191*stat_it!P191*stat_it!Q191)/(stat_it!$C161*stat_it!P161+stat_it!$C176*stat_it!P176+stat_it!$C191*stat_it!P191)</f>
-        <v>1.9348286604361371</v>
+        <v>2.2331297034085877</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1290,11 +1294,11 @@
       </c>
       <c r="P12" s="2">
         <f>(stat_it!$C162*stat_it!P162+stat_it!$C177*stat_it!P177+stat_it!$C192*stat_it!P192)/C12</f>
-        <v>65.659090909090907</v>
+        <v>97.727272727272734</v>
       </c>
       <c r="Q12" s="1">
         <f>(stat_it!$C162*stat_it!P162*stat_it!Q162+stat_it!$C177*stat_it!P177*stat_it!Q177+stat_it!$C192*stat_it!P192*stat_it!Q192)/(stat_it!$C162*stat_it!P162+stat_it!$C177*stat_it!P177+stat_it!$C192*stat_it!P192)</f>
-        <v>1.9682935271720317</v>
+        <v>2.3504651162790697</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1355,11 +1359,11 @@
       </c>
       <c r="P13" s="2">
         <f>(stat_it!$C163*stat_it!P163+stat_it!$C178*stat_it!P178+stat_it!$C193*stat_it!P193)/C13</f>
-        <v>63.355450236966824</v>
+        <v>97.905213270142184</v>
       </c>
       <c r="Q13" s="1">
         <f>(stat_it!$C163*stat_it!P163*stat_it!Q163+stat_it!$C178*stat_it!P178*stat_it!Q178+stat_it!$C193*stat_it!P193*stat_it!Q193)/(stat_it!$C163*stat_it!P163+stat_it!$C178*stat_it!P178+stat_it!$C193*stat_it!P193)</f>
-        <v>1.9712073608617593</v>
+        <v>2.1897821667150743</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1420,11 +1424,11 @@
       </c>
       <c r="P14" s="2">
         <f>(stat_it!$C164*stat_it!P164+stat_it!$C179*stat_it!P179+stat_it!$C194*stat_it!P194)/C14</f>
-        <v>46.829787234042556</v>
+        <v>97.872340425531917</v>
       </c>
       <c r="Q14" s="1">
         <f>(stat_it!$C164*stat_it!P164*stat_it!Q164+stat_it!$C179*stat_it!P179*stat_it!Q179+stat_it!$C194*stat_it!P194*stat_it!Q194)/(stat_it!$C164*stat_it!P164+stat_it!$C179*stat_it!P179+stat_it!$C194*stat_it!P194)</f>
-        <v>1.7710131758291685</v>
+        <v>1.9769565217391305</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1485,16 +1489,104 @@
       </c>
       <c r="P15" s="2">
         <f>(stat_it!$C165*stat_it!P165+stat_it!$C180*stat_it!P180+stat_it!$C195*stat_it!P195)/C15</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q15" s="1">
         <f>(stat_it!$C165*stat_it!P165*stat_it!Q165+stat_it!$C180*stat_it!P180*stat_it!Q180+stat_it!$C195*stat_it!P195*stat_it!Q195)/(stat_it!$C165*stat_it!P165+stat_it!$C180*stat_it!P180+stat_it!$C195*stat_it!P195)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C16" s="2">
+        <f>C3/C$2*100</f>
+        <v>5.7240704500978472</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:C28" si="0">C4/C$2*100</f>
+        <v>0.53816046966731901</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6908023483365948</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34246575342465752</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>4.10958904109589</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7945205479452051</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1741682974559686</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4951076320939332</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>13.698630136986301</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>2.152641878669276</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>10.322896281800391</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5988258317025439</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7847358121330719E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="2">
+        <f>(C2-SUM(C3:C15))/C2*100</f>
+        <v>47.260273972602739</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="2">
+        <f>SUM(C16:C29)</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1503,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1886553-593B-F44B-AFA8-F037AB964ECE}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1625,11 +1717,11 @@
       </c>
       <c r="P2" s="2">
         <f>IFERROR((stat_fism!$C152*stat_fism!P152+stat_fism!$C167*stat_fism!P167+stat_fism!$C182*stat_fism!P182)/C2,"-")</f>
-        <v>64.587030716723547</v>
+        <v>98.109215017064841</v>
       </c>
       <c r="Q2" s="1">
         <f>IFERROR((stat_fism!$C152*stat_fism!P152*stat_fism!Q152+stat_fism!$C167*stat_fism!P167*stat_fism!Q167+stat_fism!$C182*stat_fism!P182*stat_fism!Q182)/(stat_fism!$C152*stat_fism!P152+stat_fism!$C167*stat_fism!P167+stat_fism!$C182*stat_fism!P182),"-")</f>
-        <v>1.9134749524413444</v>
+        <v>2.1668023377165517</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1690,11 +1782,11 @@
       </c>
       <c r="P3" s="2">
         <f>IFERROR((stat_fism!$C153*stat_fism!P153+stat_fism!$C168*stat_fism!P168+stat_fism!$C183*stat_fism!P183)/C3,"-")</f>
-        <v>91.666666666666671</v>
+        <v>100</v>
       </c>
       <c r="Q3" s="1">
         <f>IFERROR((stat_fism!$C153*stat_fism!P153*stat_fism!Q153+stat_fism!$C168*stat_fism!P168*stat_fism!Q168+stat_fism!$C183*stat_fism!P183*stat_fism!Q183)/(stat_fism!$C153*stat_fism!P153+stat_fism!$C168*stat_fism!P168+stat_fism!$C183*stat_fism!P183),"-")</f>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1755,11 +1847,11 @@
       </c>
       <c r="P4" s="2">
         <f>IFERROR((stat_fism!$C154*stat_fism!P154+stat_fism!$C169*stat_fism!P169+stat_fism!$C184*stat_fism!P184)/C4,"-")</f>
-        <v>66.833333333333329</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="1">
         <f>IFERROR((stat_fism!$C154*stat_fism!P154*stat_fism!Q154+stat_fism!$C169*stat_fism!P169*stat_fism!Q169+stat_fism!$C184*stat_fism!P184*stat_fism!Q184)/(stat_fism!$C154*stat_fism!P154+stat_fism!$C169*stat_fism!P169+stat_fism!$C184*stat_fism!P184),"-")</f>
-        <v>2.2481296758104738</v>
+        <v>2.335</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1820,11 +1912,11 @@
       </c>
       <c r="P5" s="2">
         <f>IFERROR((stat_fism!$C155*stat_fism!P155+stat_fism!$C170*stat_fism!P170+stat_fism!$C185*stat_fism!P185)/C5,"-")</f>
-        <v>66.666666666666671</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="1">
         <f>IFERROR((stat_fism!$C155*stat_fism!P155*stat_fism!Q155+stat_fism!$C170*stat_fism!P170*stat_fism!Q170+stat_fism!$C185*stat_fism!P185*stat_fism!Q185)/(stat_fism!$C155*stat_fism!P155+stat_fism!$C170*stat_fism!P170+stat_fism!$C185*stat_fism!P185),"-")</f>
-        <v>1.5</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1950,11 +2042,11 @@
       </c>
       <c r="P7" s="2">
         <f>IFERROR((stat_fism!$C157*stat_fism!P157+stat_fism!$C172*stat_fism!P172+stat_fism!$C187*stat_fism!P187)/C7,"-")</f>
-        <v>68.16</v>
+        <v>100</v>
       </c>
       <c r="Q7" s="1">
         <f>IFERROR((stat_fism!$C157*stat_fism!P157*stat_fism!Q157+stat_fism!$C172*stat_fism!P172*stat_fism!Q172+stat_fism!$C187*stat_fism!P187*stat_fism!Q187)/(stat_fism!$C157*stat_fism!P157+stat_fism!$C172*stat_fism!P172+stat_fism!$C187*stat_fism!P187),"-")</f>
-        <v>1.7624882629107981</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -2015,11 +2107,11 @@
       </c>
       <c r="P8" s="2">
         <f>IFERROR((stat_fism!$C158*stat_fism!P158+stat_fism!$C173*stat_fism!P173+stat_fism!$C188*stat_fism!P188)/C8,"-")</f>
-        <v>62.5</v>
+        <v>100</v>
       </c>
       <c r="Q8" s="1">
         <f>IFERROR((stat_fism!$C158*stat_fism!P158*stat_fism!Q158+stat_fism!$C173*stat_fism!P173*stat_fism!Q173+stat_fism!$C188*stat_fism!P188*stat_fism!Q188)/(stat_fism!$C158*stat_fism!P158+stat_fism!$C173*stat_fism!P173+stat_fism!$C188*stat_fism!P188),"-")</f>
-        <v>1.8</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -2080,11 +2172,11 @@
       </c>
       <c r="P9" s="2">
         <f>IFERROR((stat_fism!$C159*stat_fism!P159+stat_fism!$C174*stat_fism!P174+stat_fism!$C189*stat_fism!P189)/C9,"-")</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="1">
         <f>IFERROR((stat_fism!$C159*stat_fism!P159*stat_fism!Q159+stat_fism!$C174*stat_fism!P174*stat_fism!Q174+stat_fism!$C189*stat_fism!P189*stat_fism!Q189)/(stat_fism!$C159*stat_fism!P159+stat_fism!$C174*stat_fism!P174+stat_fism!$C189*stat_fism!P189),"-")</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -2145,11 +2237,11 @@
       </c>
       <c r="P10" s="2">
         <f>IFERROR((stat_fism!$C160*stat_fism!P160+stat_fism!$C175*stat_fism!P175+stat_fism!$C190*stat_fism!P190)/C10,"-")</f>
-        <v>66.666666666666671</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="1">
         <f>IFERROR((stat_fism!$C160*stat_fism!P160*stat_fism!Q160+stat_fism!$C175*stat_fism!P175*stat_fism!Q175+stat_fism!$C190*stat_fism!P190*stat_fism!Q190)/(stat_fism!$C160*stat_fism!P160+stat_fism!$C175*stat_fism!P175+stat_fism!$C190*stat_fism!P190),"-")</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -2210,11 +2302,11 @@
       </c>
       <c r="P11" s="2">
         <f>IFERROR((stat_fism!$C161*stat_fism!P161+stat_fism!$C176*stat_fism!P176+stat_fism!$C191*stat_fism!P191)/C11,"-")</f>
-        <v>62.147058823529413</v>
+        <v>94.264705882352942</v>
       </c>
       <c r="Q11" s="1">
         <f>IFERROR((stat_fism!$C161*stat_fism!P161*stat_fism!Q161+stat_fism!$C176*stat_fism!P176*stat_fism!Q176+stat_fism!$C191*stat_fism!P191*stat_fism!Q191)/(stat_fism!$C161*stat_fism!P161+stat_fism!$C176*stat_fism!P176+stat_fism!$C191*stat_fism!P191),"-")</f>
-        <v>1.7137718883104589</v>
+        <v>2.0617784711388456</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -2275,11 +2367,11 @@
       </c>
       <c r="P12" s="2">
         <f>IFERROR((stat_fism!$C162*stat_fism!P162+stat_fism!$C177*stat_fism!P177+stat_fism!$C192*stat_fism!P192)/C12,"-")</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q12" s="1">
         <f>IFERROR((stat_fism!$C162*stat_fism!P162*stat_fism!Q162+stat_fism!$C177*stat_fism!P177*stat_fism!Q177+stat_fism!$C192*stat_fism!P192*stat_fism!Q192)/(stat_fism!$C162*stat_fism!P162+stat_fism!$C177*stat_fism!P177+stat_fism!$C192*stat_fism!P192),"-")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -2340,11 +2432,11 @@
       </c>
       <c r="P13" s="2">
         <f>IFERROR((stat_fism!$C163*stat_fism!P163+stat_fism!$C178*stat_fism!P178+stat_fism!$C193*stat_fism!P193)/C13,"-")</f>
-        <v>73.510204081632651</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="1">
         <f>IFERROR((stat_fism!$C163*stat_fism!P163*stat_fism!Q163+stat_fism!$C178*stat_fism!P178*stat_fism!Q178+stat_fism!$C193*stat_fism!P193*stat_fism!Q193)/(stat_fism!$C163*stat_fism!P163+stat_fism!$C178*stat_fism!P178+stat_fism!$C193*stat_fism!P193),"-")</f>
-        <v>2.249283731260411</v>
+        <v>2.6951020408163266</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -2405,11 +2497,11 @@
       </c>
       <c r="P14" s="2">
         <f>IFERROR((stat_fism!$C164*stat_fism!P164+stat_fism!$C179*stat_fism!P179+stat_fism!$C194*stat_fism!P194)/C14,"-")</f>
-        <v>71.142857142857139</v>
+        <v>100</v>
       </c>
       <c r="Q14" s="1">
         <f>IFERROR((stat_fism!$C164*stat_fism!P164*stat_fism!Q164+stat_fism!$C179*stat_fism!P179*stat_fism!Q179+stat_fism!$C194*stat_fism!P194*stat_fism!Q194)/(stat_fism!$C164*stat_fism!P164+stat_fism!$C179*stat_fism!P179+stat_fism!$C194*stat_fism!P194),"-")</f>
-        <v>1.1997991967871486</v>
+        <v>1.7114285714285715</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -2478,8 +2570,96 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C16" s="2">
+        <f>C3/C$2*100</f>
+        <v>4.0955631399317403</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:C28" si="0">C4/C$2*100</f>
+        <v>2.0477815699658701</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0238907849829351</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5324232081911262</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7303754266211606</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3651877133105803</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0238907849829351</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>11.604095563139932</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.68259385665529015</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>16.723549488054605</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7781569965870307</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="2">
+        <f>(C2-SUM(C3:C15))/C2*100</f>
+        <v>45.392491467576789</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="2">
+        <f>SUM(C16:C29)</f>
+        <v>99.999999999999986</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2487,11 +2667,196 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F0297F-8385-A04B-8B33-C27D78F343AF}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4.0955631399317403</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.7240704500978472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.0477815699658701</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.53816046966731901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.0238907849829351</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.6908023483365948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.34246575342465752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8.5324232081911262</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.10958904109589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.7303754266211606</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.7945205479452051</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.3651877133105803</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.1741682974559686</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.0238907849829351</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.4951076320939332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11.604095563139932</v>
+      </c>
+      <c r="C10" s="2">
+        <v>13.698630136986301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.68259385665529015</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.152641878669276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>16.723549488054605</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10.322896281800391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4.7781569965870307</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.5988258317025439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>9.7847358121330719E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45.392491467576789</v>
+      </c>
+      <c r="C15" s="2">
+        <v>47.260273972602739</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="C16" s="2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3C1F93-DC02-B44F-BCCF-5322294F7BE6}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D15"/>
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2666,7 +3031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C5190-69FF-6742-BDF2-BCCD5876539C}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -2692,10 +3057,10 @@
         <v>33</v>
       </c>
       <c r="B2" s="1">
-        <v>1.9134749524413444</v>
+        <v>2.1668023377165517</v>
       </c>
       <c r="C2" s="1">
-        <v>1.8659062591462141</v>
+        <v>2.0735200426764213</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2703,10 +3068,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="C3" s="1">
-        <v>1.9843764115432874</v>
+        <v>1.9680591982015736</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2714,10 +3079,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2.2481296758104738</v>
+        <v>2.335</v>
       </c>
       <c r="C4" s="1">
-        <v>2.2512468827930174</v>
+        <v>2.5560488346281911</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2725,10 +3090,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>1.5</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="C5" s="1">
-        <v>2.0900628751071735</v>
+        <v>2.4468194070080864</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2739,7 +3104,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="1">
-        <v>2.255639097744361</v>
+        <v>2.1680532445923459</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2747,10 +3112,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1.7624882629107981</v>
+        <v>1.92</v>
       </c>
       <c r="C7" s="1">
-        <v>1.5920858895705521</v>
+        <v>1.7946464646464648</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2758,10 +3123,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1.8</v>
+        <v>2.125</v>
       </c>
       <c r="C8" s="1">
-        <v>2.1491904445919046</v>
+        <v>2.6972524407252441</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2769,10 +3134,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>1.5697206303724929</v>
+        <v>1.7491666666666668</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2780,10 +3145,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>1.7765250965250967</v>
+        <v>2.1022229026331907</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2791,10 +3156,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>1.7137718883104589</v>
+        <v>2.0617784711388456</v>
       </c>
       <c r="C11" s="1">
-        <v>1.9348286604361371</v>
+        <v>2.2331297034085877</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2802,10 +3167,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>1.9682935271720317</v>
+        <v>2.3504651162790697</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2813,10 +3178,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>2.249283731260411</v>
+        <v>2.6951020408163266</v>
       </c>
       <c r="C13" s="1">
-        <v>1.9712073608617593</v>
+        <v>2.1897821667150743</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2824,10 +3189,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>1.1997991967871486</v>
+        <v>1.7114285714285715</v>
       </c>
       <c r="C14" s="1">
-        <v>1.7710131758291685</v>
+        <v>1.9769565217391305</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2838,7 +3203,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -2846,12 +3211,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C993833-F6B5-8642-90E2-9B6A7AA9195A}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3026,7 +3391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73F72A7-C305-9649-B4C9-653654303B87}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3206,12 +3571,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A8676C-9EDA-6A42-B6C2-E7400D32F918}">
   <dimension ref="A1:Q195"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="N166" sqref="N166:O166"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="P171" sqref="P171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3313,10 +3678,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -3563,10 +3928,10 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3613,10 +3978,10 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3713,10 +4078,10 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -3763,10 +4128,10 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -3813,10 +4178,10 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3863,10 +4228,10 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -3913,10 +4278,10 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4066,10 +4431,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -4216,10 +4581,10 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -4316,10 +4681,10 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -4366,10 +4731,10 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -4466,10 +4831,10 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -4516,10 +4881,10 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -4616,10 +4981,10 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -4666,10 +5031,10 @@
         <v>0</v>
       </c>
       <c r="P29">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -4716,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -4819,10 +5184,10 @@
         <v>0</v>
       </c>
       <c r="P32">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="Q32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -4969,10 +5334,10 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -5069,10 +5434,10 @@
         <v>0</v>
       </c>
       <c r="P37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -5119,10 +5484,10 @@
         <v>0</v>
       </c>
       <c r="P38">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Q38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -5219,10 +5584,10 @@
         <v>0</v>
       </c>
       <c r="P40">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -5269,10 +5634,10 @@
         <v>0</v>
       </c>
       <c r="P41">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -5319,10 +5684,10 @@
         <v>0</v>
       </c>
       <c r="P42">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Q42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -5369,10 +5734,10 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Q43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -5419,10 +5784,10 @@
         <v>0</v>
       </c>
       <c r="P44">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -5572,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="P47">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="Q47">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -5722,10 +6087,10 @@
         <v>0</v>
       </c>
       <c r="P50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -5872,10 +6237,10 @@
         <v>0</v>
       </c>
       <c r="P53">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Q53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
@@ -5972,10 +6337,10 @@
         <v>0</v>
       </c>
       <c r="P55">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6022,10 +6387,10 @@
         <v>0</v>
       </c>
       <c r="P56">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="Q56">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -6122,10 +6487,10 @@
         <v>0</v>
       </c>
       <c r="P58">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -6172,10 +6537,10 @@
         <v>0</v>
       </c>
       <c r="P59">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="Q59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -6222,10 +6587,10 @@
         <v>0</v>
       </c>
       <c r="P60">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6325,10 +6690,10 @@
         <v>0</v>
       </c>
       <c r="P62">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="Q62">
-        <v>1.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6425,10 +6790,10 @@
         <v>0</v>
       </c>
       <c r="P64">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6575,10 +6940,10 @@
         <v>0</v>
       </c>
       <c r="P67">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="Q67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -6625,10 +6990,10 @@
         <v>0</v>
       </c>
       <c r="P68">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -6675,10 +7040,10 @@
         <v>0</v>
       </c>
       <c r="P69">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
@@ -6725,10 +7090,10 @@
         <v>0</v>
       </c>
       <c r="P70">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="Q70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -6775,10 +7140,10 @@
         <v>0</v>
       </c>
       <c r="P71">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="Q71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -6875,10 +7240,10 @@
         <v>0</v>
       </c>
       <c r="P73">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="Q73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
@@ -6925,10 +7290,10 @@
         <v>0</v>
       </c>
       <c r="P74">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="Q74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -6975,10 +7340,10 @@
         <v>0</v>
       </c>
       <c r="P75">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -7078,10 +7443,10 @@
         <v>0</v>
       </c>
       <c r="P77">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="Q77">
-        <v>1.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -7178,10 +7543,10 @@
         <v>0</v>
       </c>
       <c r="P79">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
@@ -7228,10 +7593,10 @@
         <v>0</v>
       </c>
       <c r="P80">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q80">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -7328,10 +7693,10 @@
         <v>0</v>
       </c>
       <c r="P82">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="Q82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -7378,10 +7743,10 @@
         <v>0</v>
       </c>
       <c r="P83">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="Q83">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -7428,10 +7793,10 @@
         <v>0</v>
       </c>
       <c r="P84">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -7478,10 +7843,10 @@
         <v>0</v>
       </c>
       <c r="P85">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="Q85">
-        <v>1.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -7528,10 +7893,10 @@
         <v>0</v>
       </c>
       <c r="P86">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="Q86">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -7578,10 +7943,10 @@
         <v>0</v>
       </c>
       <c r="P87">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q87">
-        <v>1.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -7628,10 +7993,10 @@
         <v>0</v>
       </c>
       <c r="P88">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Q88">
-        <v>2.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -7678,10 +8043,10 @@
         <v>0</v>
       </c>
       <c r="P89">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q89">
-        <v>1.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -7728,10 +8093,10 @@
         <v>0</v>
       </c>
       <c r="P90">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -7831,10 +8196,10 @@
         <v>0.86</v>
       </c>
       <c r="P92">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="Q92">
-        <v>1.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
@@ -7981,10 +8346,10 @@
         <v>0</v>
       </c>
       <c r="P95">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q95">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
@@ -8081,10 +8446,10 @@
         <v>0</v>
       </c>
       <c r="P97">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q97">
-        <v>1.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -8131,10 +8496,10 @@
         <v>0</v>
       </c>
       <c r="P98">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="Q98">
-        <v>1.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -8181,10 +8546,10 @@
         <v>0</v>
       </c>
       <c r="P99">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
@@ -8231,10 +8596,10 @@
         <v>0</v>
       </c>
       <c r="P100">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q100">
-        <v>2.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -8281,10 +8646,10 @@
         <v>0</v>
       </c>
       <c r="P101">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="Q101">
-        <v>1.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
@@ -8331,10 +8696,10 @@
         <v>0</v>
       </c>
       <c r="P102">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q102">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
@@ -8381,10 +8746,10 @@
         <v>0</v>
       </c>
       <c r="P103">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="Q103">
-        <v>1.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -8431,10 +8796,10 @@
         <v>0.86</v>
       </c>
       <c r="P104">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Q104">
-        <v>1.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -8481,10 +8846,10 @@
         <v>0</v>
       </c>
       <c r="P105">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q105">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
@@ -8584,10 +8949,10 @@
         <v>1.82</v>
       </c>
       <c r="P107">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Q107">
-        <v>1.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
@@ -8684,10 +9049,10 @@
         <v>1.68</v>
       </c>
       <c r="P109">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q109">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -8734,10 +9099,10 @@
         <v>3.17</v>
       </c>
       <c r="P110">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="Q110">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
@@ -8834,10 +9199,10 @@
         <v>2.35</v>
       </c>
       <c r="P112">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q112">
-        <v>1.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
@@ -8884,10 +9249,10 @@
         <v>2.36</v>
       </c>
       <c r="P113">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="Q113">
-        <v>1.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
@@ -8934,10 +9299,10 @@
         <v>1.25</v>
       </c>
       <c r="P114">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q114">
-        <v>1.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
@@ -8984,10 +9349,10 @@
         <v>2.61</v>
       </c>
       <c r="P115">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="Q115">
-        <v>2.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
@@ -9034,10 +9399,10 @@
         <v>2.75</v>
       </c>
       <c r="P116">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="Q116">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -9084,10 +9449,10 @@
         <v>1.22</v>
       </c>
       <c r="P117">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="Q117">
-        <v>2.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
@@ -9134,10 +9499,10 @@
         <v>1.52</v>
       </c>
       <c r="P118">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q118">
-        <v>2.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9184,10 +9549,10 @@
         <v>1.8</v>
       </c>
       <c r="P119">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="Q119">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
@@ -9234,10 +9599,10 @@
         <v>1.74</v>
       </c>
       <c r="P120">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q120">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
@@ -9337,10 +9702,10 @@
         <v>1.99</v>
       </c>
       <c r="P122">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Q122">
-        <v>1.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
@@ -9437,10 +9802,10 @@
         <v>0.98</v>
       </c>
       <c r="P124">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q124">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
@@ -9487,10 +9852,10 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="P125">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="Q125">
-        <v>2.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
@@ -9537,10 +9902,10 @@
         <v>1.88</v>
       </c>
       <c r="P126">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
@@ -9587,10 +9952,10 @@
         <v>2.29</v>
       </c>
       <c r="P127">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="Q127">
-        <v>1.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
@@ -9637,10 +10002,10 @@
         <v>1.28</v>
       </c>
       <c r="P128">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Q128">
-        <v>2.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
@@ -9687,10 +10052,10 @@
         <v>3.43</v>
       </c>
       <c r="P129">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q129">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
@@ -9737,10 +10102,10 @@
         <v>2.81</v>
       </c>
       <c r="P130">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="Q130">
-        <v>1.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
@@ -9787,10 +10152,10 @@
         <v>3.47</v>
       </c>
       <c r="P131">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q131">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
@@ -9837,10 +10202,10 @@
         <v>0.83</v>
       </c>
       <c r="P132">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="Q132">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
@@ -9887,10 +10252,10 @@
         <v>1.5</v>
       </c>
       <c r="P133">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="Q133">
-        <v>1.77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
@@ -9937,10 +10302,10 @@
         <v>1.76</v>
       </c>
       <c r="P134">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q134">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
@@ -10090,10 +10455,10 @@
         <v>2.65</v>
       </c>
       <c r="P137">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q137">
-        <v>1.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
@@ -10190,10 +10555,10 @@
         <v>0.85</v>
       </c>
       <c r="P139">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q139">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
@@ -10240,10 +10605,10 @@
         <v>3.72</v>
       </c>
       <c r="P140">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="Q140">
-        <v>1.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
@@ -10290,10 +10655,10 @@
         <v>2.76</v>
       </c>
       <c r="P141">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q141">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
@@ -10340,10 +10705,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="P142">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q142">
-        <v>1.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
@@ -10390,10 +10755,10 @@
         <v>1.97</v>
       </c>
       <c r="P143">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="Q143">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
@@ -10440,10 +10805,10 @@
         <v>6.13</v>
       </c>
       <c r="P144">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q144">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
@@ -10490,10 +10855,10 @@
         <v>1.35</v>
       </c>
       <c r="P145">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q145">
-        <v>1.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
@@ -10540,10 +10905,10 @@
         <v>2.12</v>
       </c>
       <c r="P146">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="Q146">
-        <v>1.83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -10590,10 +10955,10 @@
         <v>3.8</v>
       </c>
       <c r="P147">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q147">
-        <v>2.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
@@ -10640,10 +11005,10 @@
         <v>2.92</v>
       </c>
       <c r="P148">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="Q148">
-        <v>2.0299999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -10690,10 +11055,10 @@
         <v>1.97</v>
       </c>
       <c r="P149">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="Q149">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
@@ -10740,10 +11105,10 @@
         <v>1.53</v>
       </c>
       <c r="P150">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
@@ -10843,10 +11208,10 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="P152">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="Q152">
-        <v>1.49</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
@@ -10943,10 +11308,10 @@
         <v>1.81</v>
       </c>
       <c r="P154">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="Q154">
-        <v>1.5</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -10993,10 +11358,10 @@
         <v>9.65</v>
       </c>
       <c r="P155">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="Q155">
-        <v>1.43</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
@@ -11043,10 +11408,10 @@
         <v>3.77</v>
       </c>
       <c r="P156">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
@@ -11093,10 +11458,10 @@
         <v>1.54</v>
       </c>
       <c r="P157">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="Q157">
-        <v>1.38</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
@@ -11143,10 +11508,10 @@
         <v>2.11</v>
       </c>
       <c r="P158">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q158">
-        <v>1.42</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
@@ -11193,10 +11558,10 @@
         <v>1.56</v>
       </c>
       <c r="P159">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="Q159">
-        <v>1.33</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
@@ -11243,10 +11608,10 @@
         <v>1.26</v>
       </c>
       <c r="P160">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="Q160">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
@@ -11293,10 +11658,10 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="P161">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="Q161">
-        <v>1.64</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
@@ -11343,10 +11708,10 @@
         <v>1.4</v>
       </c>
       <c r="P162">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="Q162">
-        <v>1.6</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
@@ -11393,10 +11758,10 @@
         <v>2.34</v>
       </c>
       <c r="P163">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="Q163">
-        <v>1.47</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
@@ -11443,10 +11808,10 @@
         <v>3.45</v>
       </c>
       <c r="P164">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="Q164">
-        <v>1.6</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
@@ -11596,10 +11961,10 @@
         <v>2.33</v>
       </c>
       <c r="P167">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="Q167">
-        <v>1.39</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
@@ -11646,10 +12011,10 @@
         <v>5.08</v>
       </c>
       <c r="P168">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="Q168">
-        <v>1</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
@@ -11699,7 +12064,7 @@
         <v>80</v>
       </c>
       <c r="Q169">
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
@@ -11746,10 +12111,10 @@
         <v>6.73</v>
       </c>
       <c r="P170">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="Q170">
-        <v>1.17</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
@@ -11796,10 +12161,10 @@
         <v>2.35</v>
       </c>
       <c r="P171">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="Q171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
@@ -11846,10 +12211,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="P172">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="Q172">
-        <v>1.37</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
@@ -11896,10 +12261,10 @@
         <v>1.86</v>
       </c>
       <c r="P173">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="Q173">
-        <v>1.5</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
@@ -11946,10 +12311,10 @@
         <v>1.79</v>
       </c>
       <c r="P174">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="Q174">
-        <v>1.4</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
@@ -11996,10 +12361,10 @@
         <v>3.23</v>
       </c>
       <c r="P175">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="Q175">
-        <v>1</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -12046,10 +12411,10 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="P176">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="Q176">
-        <v>1.5</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.2">
@@ -12096,10 +12461,10 @@
         <v>1.47</v>
       </c>
       <c r="P177">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="Q177">
-        <v>1.6</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.2">
@@ -12146,10 +12511,10 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="P178">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="Q178">
-        <v>1.65</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.2">
@@ -12196,10 +12561,10 @@
         <v>1.78</v>
       </c>
       <c r="P179">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="Q179">
-        <v>1.18</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">
@@ -12246,10 +12611,10 @@
         <v>1.07</v>
       </c>
       <c r="P180">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q180">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.2">
@@ -13010,12 +13375,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3674CC-13DA-CC4F-BB28-17C140C0B3A8}">
   <dimension ref="A1:Q195"/>
   <sheetViews>
-    <sheetView topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:Q195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14623,10 +14988,10 @@
         <v>0</v>
       </c>
       <c r="P32">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="Q32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -14923,10 +15288,10 @@
         <v>0</v>
       </c>
       <c r="P38">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -15023,10 +15388,10 @@
         <v>0</v>
       </c>
       <c r="P40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -15073,10 +15438,10 @@
         <v>0</v>
       </c>
       <c r="P41">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -15376,10 +15741,10 @@
         <v>0</v>
       </c>
       <c r="P47">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -15776,10 +16141,10 @@
         <v>0</v>
       </c>
       <c r="P55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -15826,10 +16191,10 @@
         <v>0</v>
       </c>
       <c r="P56">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="Q56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -16129,10 +16494,10 @@
         <v>0</v>
       </c>
       <c r="P62">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="Q62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -16279,10 +16644,10 @@
         <v>0</v>
       </c>
       <c r="P65">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -16529,10 +16894,10 @@
         <v>0</v>
       </c>
       <c r="P70">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -16579,10 +16944,10 @@
         <v>0</v>
       </c>
       <c r="P71">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -16679,10 +17044,10 @@
         <v>0</v>
       </c>
       <c r="P73">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
@@ -16729,10 +17094,10 @@
         <v>0</v>
       </c>
       <c r="P74">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -16882,10 +17247,10 @@
         <v>0</v>
       </c>
       <c r="P77">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="Q77">
-        <v>1.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -17032,10 +17397,10 @@
         <v>0</v>
       </c>
       <c r="P80">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q80">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -17282,10 +17647,10 @@
         <v>0</v>
       </c>
       <c r="P85">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -17332,10 +17697,10 @@
         <v>0</v>
       </c>
       <c r="P86">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q86">
-        <v>1.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -17432,10 +17797,10 @@
         <v>0</v>
       </c>
       <c r="P88">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="Q88">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -17482,10 +17847,10 @@
         <v>0</v>
       </c>
       <c r="P89">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -17532,10 +17897,10 @@
         <v>0</v>
       </c>
       <c r="P90">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -17635,10 +18000,10 @@
         <v>0.68</v>
       </c>
       <c r="P92">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="Q92">
-        <v>1.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
@@ -17785,10 +18150,10 @@
         <v>0</v>
       </c>
       <c r="P95">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
@@ -17885,10 +18250,10 @@
         <v>0</v>
       </c>
       <c r="P97">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q97">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -17935,10 +18300,10 @@
         <v>0</v>
       </c>
       <c r="P98">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q98">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -18035,10 +18400,10 @@
         <v>0</v>
       </c>
       <c r="P100">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q100">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -18085,10 +18450,10 @@
         <v>0</v>
       </c>
       <c r="P101">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="Q101">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
@@ -18185,10 +18550,10 @@
         <v>0</v>
       </c>
       <c r="P103">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q103">
-        <v>1.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -18235,10 +18600,10 @@
         <v>0.86</v>
       </c>
       <c r="P104">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q104">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -18388,10 +18753,10 @@
         <v>1.91</v>
       </c>
       <c r="P107">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Q107">
-        <v>1.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
@@ -18538,10 +18903,10 @@
         <v>5.18</v>
       </c>
       <c r="P110">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q110">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
@@ -18638,10 +19003,10 @@
         <v>2.42</v>
       </c>
       <c r="P112">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q112">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
@@ -18688,10 +19053,10 @@
         <v>0</v>
       </c>
       <c r="P113">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q113">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
@@ -18738,10 +19103,10 @@
         <v>1.54</v>
       </c>
       <c r="P114">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q114">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
@@ -18788,10 +19153,10 @@
         <v>3.09</v>
       </c>
       <c r="P115">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q115">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
@@ -18838,10 +19203,10 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="P116">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="Q116">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -18888,10 +19253,10 @@
         <v>2.54</v>
       </c>
       <c r="P117">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q117">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
@@ -18938,10 +19303,10 @@
         <v>1.52</v>
       </c>
       <c r="P118">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="Q118">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -18988,10 +19353,10 @@
         <v>2.79</v>
       </c>
       <c r="P119">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="Q119">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
@@ -19141,10 +19506,10 @@
         <v>1.76</v>
       </c>
       <c r="P122">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="Q122">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
@@ -19241,10 +19606,10 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="P124">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q124">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
@@ -19291,10 +19656,10 @@
         <v>1.28</v>
       </c>
       <c r="P125">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
@@ -19391,10 +19756,10 @@
         <v>2.27</v>
       </c>
       <c r="P127">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="Q127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
@@ -19591,10 +19956,10 @@
         <v>2.82</v>
       </c>
       <c r="P131">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="Q131">
-        <v>2.2200000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
@@ -19691,10 +20056,10 @@
         <v>0.96</v>
       </c>
       <c r="P133">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q133">
-        <v>1.83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
@@ -19741,10 +20106,10 @@
         <v>2.09</v>
       </c>
       <c r="P134">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q134">
-        <v>1.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
@@ -19894,10 +20259,10 @@
         <v>2.87</v>
       </c>
       <c r="P137">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="Q137">
-        <v>1.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
@@ -19994,10 +20359,10 @@
         <v>0.71</v>
       </c>
       <c r="P139">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q139">
-        <v>2.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
@@ -20044,10 +20409,10 @@
         <v>8.3800000000000008</v>
       </c>
       <c r="P140">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q140">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
@@ -20144,10 +20509,10 @@
         <v>3</v>
       </c>
       <c r="P142">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
@@ -20194,10 +20559,10 @@
         <v>1.84</v>
       </c>
       <c r="P143">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="Q143">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
@@ -20344,10 +20709,10 @@
         <v>2.81</v>
       </c>
       <c r="P146">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q146">
-        <v>2.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -20394,10 +20759,10 @@
         <v>1.93</v>
       </c>
       <c r="P147">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q147">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
@@ -20444,10 +20809,10 @@
         <v>2.98</v>
       </c>
       <c r="P148">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q148">
-        <v>2.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -20494,10 +20859,10 @@
         <v>3.7</v>
       </c>
       <c r="P149">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q149">
-        <v>1.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
@@ -20647,10 +21012,10 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="P152">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="Q152">
-        <v>1.53</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
@@ -20747,10 +21112,10 @@
         <v>2.5</v>
       </c>
       <c r="P154">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q154">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -20797,10 +21162,10 @@
         <v>1.45</v>
       </c>
       <c r="P155">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q155">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
@@ -20897,10 +21262,10 @@
         <v>1.5</v>
       </c>
       <c r="P157">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q157">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
@@ -20947,10 +21312,10 @@
         <v>1.64</v>
       </c>
       <c r="P158">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q158">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
@@ -20997,10 +21362,10 @@
         <v>2.04</v>
       </c>
       <c r="P159">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
@@ -21050,7 +21415,7 @@
         <v>100</v>
       </c>
       <c r="Q160">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
@@ -21097,10 +21462,10 @@
         <v>1.47</v>
       </c>
       <c r="P161">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="Q161">
-        <v>1.2</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
@@ -21147,10 +21512,10 @@
         <v>0.16</v>
       </c>
       <c r="P162">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q162">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
@@ -21197,10 +21562,10 @@
         <v>2.9</v>
       </c>
       <c r="P163">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="Q163">
-        <v>1.89</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
@@ -21247,10 +21612,10 @@
         <v>1.87</v>
       </c>
       <c r="P164">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="Q164">
-        <v>2</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
@@ -21400,10 +21765,10 @@
         <v>1.95</v>
       </c>
       <c r="P167">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="Q167">
-        <v>1.6</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
@@ -21450,10 +21815,10 @@
         <v>12.68</v>
       </c>
       <c r="P168">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q168">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
@@ -21500,10 +21865,10 @@
         <v>2.58</v>
       </c>
       <c r="P169">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="Q169">
-        <v>1.5</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
@@ -21553,7 +21918,7 @@
         <v>100</v>
       </c>
       <c r="Q170">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
@@ -21650,10 +22015,10 @@
         <v>1.42</v>
       </c>
       <c r="P172">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="Q172">
-        <v>1.57</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
@@ -21700,10 +22065,10 @@
         <v>0.5</v>
       </c>
       <c r="P173">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q173">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
@@ -21750,7 +22115,7 @@
         <v>1.83</v>
       </c>
       <c r="P174">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q174">
         <v>2</v>
@@ -21800,10 +22165,10 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="P175">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q175">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -21850,10 +22215,10 @@
         <v>2.42</v>
       </c>
       <c r="P176">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="Q176">
-        <v>1.6</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.2">
@@ -21903,7 +22268,7 @@
         <v>100</v>
       </c>
       <c r="Q177">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.2">
@@ -21950,10 +22315,10 @@
         <v>1.46</v>
       </c>
       <c r="P178">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="Q178">
-        <v>2.08</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.2">
@@ -22000,10 +22365,10 @@
         <v>1.42</v>
       </c>
       <c r="P179">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="Q179">
-        <v>1</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>